<commit_message>
corrigi planilha principal e refiz figuras
Fiz uma pequena correção na planilha principal.  Também modifiquei as figuras para ficar de acordo com o manuscrito. Além disso também refiz os calculos de ENN_MN
</commit_message>
<xml_diff>
--- a/data/planilha_metricas.xlsx
+++ b/data/planilha_metricas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Alencar\OneDrive\Documentos\Mestrado\INPE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lucas_alencar\github\defpatt_reg\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_6E924FA58DB750B09341C4D4FCF798E3D51CAAFF" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765EBF15-1F09-4504-8BEF-6CE117FADDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1770" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="5445" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metricas_prima" sheetId="7" r:id="rId1"/>
@@ -32,9 +32,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="145">
   <si>
     <t>22568_1985</t>
-  </si>
-  <si>
-    <t>paisagem_ano</t>
   </si>
   <si>
     <t>22568_1990</t>
@@ -137,27 +134,6 @@
   </si>
   <si>
     <t>22668_2015</t>
-  </si>
-  <si>
-    <t>22668_2_1985</t>
-  </si>
-  <si>
-    <t>22668_2_1990</t>
-  </si>
-  <si>
-    <t>22668_2_1995</t>
-  </si>
-  <si>
-    <t>22668_2_2000</t>
-  </si>
-  <si>
-    <t>22668_2_2005</t>
-  </si>
-  <si>
-    <t>22668_2_2010</t>
-  </si>
-  <si>
-    <t>22668_2_2015</t>
   </si>
   <si>
     <t>23069_1985</t>
@@ -337,48 +313,6 @@
     <t>22863_2015</t>
   </si>
   <si>
-    <t>23267_2_1985</t>
-  </si>
-  <si>
-    <t>23267_2_1990</t>
-  </si>
-  <si>
-    <t>23267_2_1995</t>
-  </si>
-  <si>
-    <t>23267_2_2000</t>
-  </si>
-  <si>
-    <t>23267_2_2005</t>
-  </si>
-  <si>
-    <t>23267_2_2010</t>
-  </si>
-  <si>
-    <t>23267_2_2015</t>
-  </si>
-  <si>
-    <t>23069_2_1985</t>
-  </si>
-  <si>
-    <t>23069_2_1990</t>
-  </si>
-  <si>
-    <t>23069_2_1995</t>
-  </si>
-  <si>
-    <t>23069_2_2000</t>
-  </si>
-  <si>
-    <t>23069_2_2005</t>
-  </si>
-  <si>
-    <t>23069_2_2010</t>
-  </si>
-  <si>
-    <t>23069_2_2015</t>
-  </si>
-  <si>
     <t>areaha_florprima</t>
   </si>
   <si>
@@ -465,6 +399,72 @@
   <si>
     <t>MT</t>
   </si>
+  <si>
+    <t>226682_1985</t>
+  </si>
+  <si>
+    <t>226682_1990</t>
+  </si>
+  <si>
+    <t>226682_1995</t>
+  </si>
+  <si>
+    <t>226682_2000</t>
+  </si>
+  <si>
+    <t>226682_2005</t>
+  </si>
+  <si>
+    <t>226682_2010</t>
+  </si>
+  <si>
+    <t>226682_2015</t>
+  </si>
+  <si>
+    <t>230692_1985</t>
+  </si>
+  <si>
+    <t>230692_1990</t>
+  </si>
+  <si>
+    <t>230692_1995</t>
+  </si>
+  <si>
+    <t>230692_2000</t>
+  </si>
+  <si>
+    <t>230692_2005</t>
+  </si>
+  <si>
+    <t>230692_2010</t>
+  </si>
+  <si>
+    <t>230692_2015</t>
+  </si>
+  <si>
+    <t>232672_1985</t>
+  </si>
+  <si>
+    <t>232672_1990</t>
+  </si>
+  <si>
+    <t>232672_1995</t>
+  </si>
+  <si>
+    <t>232672_2000</t>
+  </si>
+  <si>
+    <t>232672_2005</t>
+  </si>
+  <si>
+    <t>232672_2010</t>
+  </si>
+  <si>
+    <t>232672_2015</t>
+  </si>
+  <si>
+    <t>paisagem_ano</t>
+  </si>
 </sst>
 </file>
 
@@ -525,7 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -549,6 +549,7 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -891,10 +892,10 @@
   <dimension ref="A1:AK99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1:W1048576"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,130 +930,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>1</v>
+      <c r="A1" s="13" t="s">
+        <v>144</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>90</v>
-      </c>
       <c r="V1" s="7" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="Y1" s="7" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Z1" s="7" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="AB1" s="7" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="AC1" s="7" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="AD1" s="7" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="AE1" s="7" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="AF1" s="7" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="AG1" s="7" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="AH1" s="7" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="AI1" s="7" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="AJ1" s="7" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="AK1" s="7" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="7">
         <v>1985</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E2" s="8">
         <v>200612.83499999999</v>
@@ -1154,16 +1155,16 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="7">
         <v>1990</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E3" s="8">
         <v>195781.36499999999</v>
@@ -1265,16 +1266,16 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="7">
         <v>1995</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E4" s="8">
         <v>175073.67</v>
@@ -1376,16 +1377,16 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>2000</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E5" s="8">
         <v>146707.20000000001</v>
@@ -1487,16 +1488,16 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>2005</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E6" s="8">
         <v>82508.535000000003</v>
@@ -1598,16 +1599,16 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>2010</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E7" s="8">
         <v>59145.66</v>
@@ -1709,16 +1710,16 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>2015</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E8" s="8">
         <v>42556.184999999998</v>
@@ -1826,10 +1827,10 @@
         <v>1985</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E9" s="8">
         <v>217841.89679999999</v>
@@ -1931,16 +1932,16 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="7">
         <v>1990</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E10" s="8">
         <v>204314.5827</v>
@@ -2042,16 +2043,16 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="7">
         <v>1995</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E11" s="8">
         <v>195377.24789999999</v>
@@ -2153,16 +2154,16 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>2000</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E12" s="8">
         <v>180084.27420000001</v>
@@ -2264,16 +2265,16 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>2005</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E13" s="8">
         <v>163588.17240000001</v>
@@ -2375,16 +2376,16 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>2010</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E14" s="8">
         <v>154111.33170000001</v>
@@ -2486,16 +2487,16 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>2015</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E15" s="8">
         <v>153658.44810000001</v>
@@ -2597,16 +2598,16 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="7">
         <v>1985</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E16" s="8">
         <v>240909.3</v>
@@ -2708,16 +2709,16 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="7">
         <v>1990</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E17" s="8">
         <v>237120.88500000001</v>
@@ -2819,16 +2820,16 @@
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="7">
         <v>1995</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D18" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E18" s="8">
         <v>232115.85</v>
@@ -2930,16 +2931,16 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19">
         <v>2000</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E19" s="8">
         <v>225677.25</v>
@@ -3041,16 +3042,16 @@
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20">
         <v>2005</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E20" s="8">
         <v>187118.82</v>
@@ -3152,16 +3153,16 @@
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21">
         <v>2010</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E21" s="8">
         <v>181220.08499999999</v>
@@ -3263,16 +3264,16 @@
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22">
         <v>2015</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E22" s="8">
         <v>173868.70499999999</v>
@@ -3373,17 +3374,17 @@
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>36</v>
+      <c r="A23" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="B23" s="7">
         <v>1985</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E23" s="8">
         <v>210114.36</v>
@@ -3484,17 +3485,17 @@
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>37</v>
+      <c r="A24" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="B24" s="7">
         <v>1990</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D24" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E24" s="8">
         <v>199544.94</v>
@@ -3595,17 +3596,17 @@
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>38</v>
+      <c r="A25" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="B25" s="7">
         <v>1995</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E25" s="8">
         <v>187107.3</v>
@@ -3706,17 +3707,17 @@
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>39</v>
+      <c r="A26" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="B26">
         <v>2000</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E26" s="8">
         <v>168636.33</v>
@@ -3817,17 +3818,17 @@
       </c>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>40</v>
+      <c r="A27" s="13" t="s">
+        <v>127</v>
       </c>
       <c r="B27">
         <v>2005</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D27" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E27" s="8">
         <v>154341.63</v>
@@ -3928,17 +3929,17 @@
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>41</v>
+      <c r="A28" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="B28">
         <v>2010</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E28" s="8">
         <v>152333.01</v>
@@ -4039,17 +4040,17 @@
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>42</v>
+      <c r="A29" s="13" t="s">
+        <v>129</v>
       </c>
       <c r="B29">
         <v>2015</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E29" s="8">
         <v>147368.43</v>
@@ -4151,16 +4152,16 @@
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" s="7">
         <v>1985</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D30" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E30" s="8">
         <v>234822.375</v>
@@ -4214,7 +4215,7 @@
         <v>162116.92938165271</v>
       </c>
       <c r="V30" s="7" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="W30" s="7">
         <v>234.69810000000001</v>
@@ -4262,16 +4263,16 @@
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="7">
         <v>1990</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E31" s="8">
         <v>225753.16500000001</v>
@@ -4373,16 +4374,16 @@
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" s="7">
         <v>1995</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D32" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E32" s="8">
         <v>212744.61</v>
@@ -4484,16 +4485,16 @@
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33">
         <v>2000</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E33" s="8">
         <v>192123.72</v>
@@ -4595,16 +4596,16 @@
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34">
         <v>2005</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D34" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E34" s="8">
         <v>122615.28</v>
@@ -4706,16 +4707,16 @@
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35">
         <v>2010</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E35" s="8">
         <v>111851.1</v>
@@ -4817,16 +4818,16 @@
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36">
         <v>2015</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E36" s="8">
         <v>108271.53</v>
@@ -4928,16 +4929,16 @@
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" s="7">
         <v>1985</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D37" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E37" s="10">
         <v>231680.38500000001</v>
@@ -5039,16 +5040,16 @@
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" s="7">
         <v>1990</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E38" s="10">
         <v>224707.27499999999</v>
@@ -5150,16 +5151,16 @@
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" s="7">
         <v>1995</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E39" s="10">
         <v>211046.35500000001</v>
@@ -5261,16 +5262,16 @@
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40">
         <v>2000</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E40" s="10">
         <v>180611.82</v>
@@ -5372,16 +5373,16 @@
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41">
         <v>2005</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D41" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E41" s="10">
         <v>154130.31</v>
@@ -5483,16 +5484,16 @@
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B42">
         <v>2010</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E42" s="10">
         <v>148172.67000000001</v>
@@ -5594,16 +5595,16 @@
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B43">
         <v>2015</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E43" s="10">
         <v>146404.39499999999</v>
@@ -5704,17 +5705,17 @@
       </c>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>109</v>
+      <c r="A44" s="13" t="s">
+        <v>130</v>
       </c>
       <c r="B44" s="7">
         <v>1985</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E44" s="8">
         <v>217665.54</v>
@@ -5815,17 +5816,17 @@
       </c>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>110</v>
+      <c r="A45" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="B45" s="7">
         <v>1990</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E45" s="8">
         <v>158865.52079830199</v>
@@ -5926,17 +5927,17 @@
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>111</v>
+      <c r="A46" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="B46" s="7">
         <v>1995</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E46" s="8">
         <v>106253.73</v>
@@ -6037,17 +6038,17 @@
       </c>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>112</v>
+      <c r="A47" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="B47">
         <v>2000</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D47" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E47" s="8">
         <v>90627.12</v>
@@ -6148,17 +6149,17 @@
       </c>
     </row>
     <row r="48" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>113</v>
+      <c r="A48" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="B48">
         <v>2005</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E48" s="8">
         <v>81960.12</v>
@@ -6259,17 +6260,17 @@
       </c>
     </row>
     <row r="49" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>114</v>
+      <c r="A49" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="B49">
         <v>2010</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E49" s="8">
         <v>80694.494999999995</v>
@@ -6370,17 +6371,17 @@
       </c>
     </row>
     <row r="50" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>115</v>
+      <c r="A50" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="B50">
         <v>2015</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E50" s="8">
         <v>80798.67</v>
@@ -6482,16 +6483,16 @@
     </row>
     <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B51" s="7">
         <v>1985</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D51" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E51" s="8">
         <v>211742.16209999999</v>
@@ -6593,16 +6594,16 @@
     </row>
     <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B52" s="7">
         <v>1990</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D52" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E52" s="11">
         <v>184419.27674999999</v>
@@ -6704,16 +6705,16 @@
     </row>
     <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B53" s="7">
         <v>1995</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D53" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E53" s="11">
         <v>165229.72154999999</v>
@@ -6815,16 +6816,16 @@
     </row>
     <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B54">
         <v>2000</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D54" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E54" s="11">
         <v>129699.6516</v>
@@ -6926,16 +6927,16 @@
     </row>
     <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B55">
         <v>2005</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D55" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E55" s="11">
         <v>105869.0034</v>
@@ -7037,16 +7038,16 @@
     </row>
     <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B56">
         <v>2010</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D56" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E56" s="11">
         <v>81728.553599999999</v>
@@ -7148,16 +7149,16 @@
     </row>
     <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B57">
         <v>2015</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D57" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E57" s="11">
         <v>79279.7886</v>
@@ -7259,16 +7260,16 @@
     </row>
     <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B58" s="7">
         <v>1985</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D58" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E58" s="8">
         <v>231270.48</v>
@@ -7370,16 +7371,16 @@
     </row>
     <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B59" s="7">
         <v>1990</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E59" s="8">
         <v>218837.79</v>
@@ -7481,16 +7482,16 @@
     </row>
     <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B60" s="7">
         <v>1995</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D60" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E60" s="8">
         <v>206185.54500000001</v>
@@ -7592,16 +7593,16 @@
     </row>
     <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B61">
         <v>2000</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D61" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E61" s="8">
         <v>194848.74</v>
@@ -7703,16 +7704,16 @@
     </row>
     <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B62">
         <v>2005</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D62" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E62" s="8">
         <v>176668.74</v>
@@ -7814,16 +7815,16 @@
     </row>
     <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B63">
         <v>2010</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E63" s="8">
         <v>159521.04</v>
@@ -7925,16 +7926,16 @@
     </row>
     <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B64">
         <v>2015</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D64" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E64" s="8">
         <v>148544.73000000001</v>
@@ -8036,16 +8037,16 @@
     </row>
     <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B65" s="7">
         <v>1985</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D65" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E65" s="10">
         <v>204157.935</v>
@@ -8147,16 +8148,16 @@
     </row>
     <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B66" s="7">
         <v>1990</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D66" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E66" s="10">
         <v>150250.14000000001</v>
@@ -8258,16 +8259,16 @@
     </row>
     <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B67" s="7">
         <v>1995</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D67" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E67" s="10">
         <v>85294.792499999996</v>
@@ -8369,16 +8370,16 @@
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B68">
         <v>2000</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E68" s="10">
         <v>80497.214999999997</v>
@@ -8480,16 +8481,16 @@
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B69">
         <v>2005</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D69" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E69" s="10">
         <v>57521.565000000002</v>
@@ -8591,16 +8592,16 @@
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B70">
         <v>2010</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D70" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E70" s="10">
         <v>49668.84</v>
@@ -8702,16 +8703,16 @@
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B71">
         <v>2015</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E71" s="10">
         <v>45849.599999999999</v>
@@ -8813,16 +8814,16 @@
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B72" s="7">
         <v>1985</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D72" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E72" s="8">
         <v>235254.51</v>
@@ -8924,16 +8925,16 @@
     </row>
     <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B73" s="7">
         <v>1990</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D73" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E73" s="8">
         <v>226563.16500000001</v>
@@ -9035,16 +9036,16 @@
     </row>
     <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B74" s="7">
         <v>1995</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D74" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E74" s="8">
         <v>216473.58</v>
@@ -9146,16 +9147,16 @@
     </row>
     <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B75">
         <v>2000</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D75" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E75" s="8">
         <v>204042.6</v>
@@ -9257,16 +9258,16 @@
     </row>
     <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B76">
         <v>2005</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D76" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E76" s="8">
         <v>186080.85</v>
@@ -9368,16 +9369,16 @@
     </row>
     <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B77">
         <v>2010</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D77" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E77" s="8">
         <v>161910.9</v>
@@ -9479,16 +9480,16 @@
     </row>
     <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B78">
         <v>2015</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D78" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E78" s="8">
         <v>154905.97500000001</v>
@@ -9590,16 +9591,16 @@
     </row>
     <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B79" s="7">
         <v>1985</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D79" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E79" s="8">
         <v>230801.59</v>
@@ -9701,16 +9702,16 @@
     </row>
     <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B80" s="7">
         <v>1990</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D80" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E80" s="8">
         <v>214581.62</v>
@@ -9812,16 +9813,16 @@
     </row>
     <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B81" s="7">
         <v>1995</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D81" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E81" s="8">
         <v>169014.16999999899</v>
@@ -9923,16 +9924,16 @@
     </row>
     <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B82">
         <v>2000</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D82" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E82" s="8">
         <v>111587.27</v>
@@ -10034,16 +10035,16 @@
     </row>
     <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B83">
         <v>2005</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D83" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E83" s="8">
         <v>71052.800000000294</v>
@@ -10145,16 +10146,16 @@
     </row>
     <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B84">
         <v>2010</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D84" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E84" s="8">
         <v>60164.020000000099</v>
@@ -10256,16 +10257,16 @@
     </row>
     <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B85">
         <v>2015</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D85" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E85" s="8">
         <v>54811.500000000102</v>
@@ -10367,16 +10368,16 @@
     </row>
     <row r="86" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B86" s="7">
         <v>1985</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D86" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E86" s="8">
         <v>229369.59</v>
@@ -10478,16 +10479,16 @@
     </row>
     <row r="87" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B87" s="7">
         <v>1990</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D87" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E87" s="8">
         <v>198771.21</v>
@@ -10589,16 +10590,16 @@
     </row>
     <row r="88" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B88" s="7">
         <v>1995</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D88" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E88" s="8">
         <v>162480.95999999999</v>
@@ -10700,16 +10701,16 @@
     </row>
     <row r="89" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B89">
         <v>2000</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D89" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E89" s="8">
         <v>162480.95999999999</v>
@@ -10811,16 +10812,16 @@
     </row>
     <row r="90" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B90">
         <v>2005</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D90" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E90" s="8">
         <v>107127.63</v>
@@ -10922,16 +10923,16 @@
     </row>
     <row r="91" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B91">
         <v>2010</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D91" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E91" s="8">
         <v>90770.03</v>
@@ -11033,16 +11034,16 @@
     </row>
     <row r="92" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B92">
         <v>2015</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D92" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E92" s="8">
         <v>76870.89</v>
@@ -11143,17 +11144,17 @@
       </c>
     </row>
     <row r="93" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A93" s="7" t="s">
-        <v>102</v>
+      <c r="A93" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="B93" s="7">
         <v>1985</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D93" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E93" s="8">
         <v>222511.95</v>
@@ -11254,17 +11255,17 @@
       </c>
     </row>
     <row r="94" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
-        <v>103</v>
+      <c r="A94" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="B94" s="7">
         <v>1990</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D94" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E94" s="8">
         <v>191158.83</v>
@@ -11365,17 +11366,17 @@
       </c>
     </row>
     <row r="95" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A95" s="7" t="s">
-        <v>104</v>
+      <c r="A95" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="B95" s="7">
         <v>1995</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D95" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E95" s="8">
         <v>162731.79</v>
@@ -11476,17 +11477,17 @@
       </c>
     </row>
     <row r="96" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A96" s="7" t="s">
-        <v>105</v>
+      <c r="A96" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="B96">
         <v>2000</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D96" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E96" s="8">
         <v>134795.47500000001</v>
@@ -11587,17 +11588,17 @@
       </c>
     </row>
     <row r="97" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A97" s="7" t="s">
-        <v>106</v>
+      <c r="A97" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="B97">
         <v>2005</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D97" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E97" s="8">
         <v>93254.535000000003</v>
@@ -11698,17 +11699,17 @@
       </c>
     </row>
     <row r="98" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
-        <v>107</v>
+      <c r="A98" s="13" t="s">
+        <v>142</v>
       </c>
       <c r="B98">
         <v>2010</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D98" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E98" s="8">
         <v>83457.45</v>
@@ -11809,17 +11810,17 @@
       </c>
     </row>
     <row r="99" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A99" s="7" t="s">
-        <v>108</v>
+      <c r="A99" s="13" t="s">
+        <v>143</v>
       </c>
       <c r="B99">
         <v>2015</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D99" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E99" s="8">
         <v>74312.19</v>
@@ -11933,10 +11934,10 @@
   <dimension ref="A1:AK120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X2" sqref="X2:X99"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11968,129 +11969,129 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="G1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" t="s">
+      <c r="R1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" t="s">
         <v>79</v>
       </c>
-      <c r="I1" t="s">
+      <c r="T1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" t="s">
+      <c r="U1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" t="s">
+      <c r="V1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" t="s">
-        <v>86</v>
-      </c>
-      <c r="O1" t="s">
-        <v>91</v>
-      </c>
-      <c r="P1" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R1" t="s">
-        <v>94</v>
-      </c>
-      <c r="S1" t="s">
-        <v>87</v>
-      </c>
-      <c r="T1" t="s">
-        <v>88</v>
-      </c>
-      <c r="U1" t="s">
-        <v>89</v>
-      </c>
-      <c r="V1" t="s">
-        <v>90</v>
-      </c>
       <c r="W1" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="X1" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="Y1" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="Z1" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="AA1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="AB1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="AC1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="AD1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="AE1" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="AF1" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="AG1" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="AH1" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="AI1" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="AJ1" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="AK1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C2" s="7">
         <v>1985</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E2" s="2">
         <v>205013.655</v>
@@ -12195,16 +12196,16 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C3" s="7">
         <v>1990</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E3" s="2">
         <v>208251.315</v>
@@ -12309,16 +12310,16 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C4" s="7">
         <v>1995</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E4" s="2">
         <v>194066.685</v>
@@ -12423,16 +12424,16 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C5">
         <v>2000</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E5" s="2">
         <v>164930.49</v>
@@ -12537,16 +12538,16 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C6">
         <v>2005</v>
       </c>
       <c r="D6" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E6" s="2">
         <v>119833.785</v>
@@ -12651,16 +12652,16 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C7">
         <v>2010</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E7" s="2">
         <v>87651.044999999998</v>
@@ -12765,16 +12766,16 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C8">
         <v>2015</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E8" s="2">
         <v>59695.425000000003</v>
@@ -12882,13 +12883,13 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C9" s="7">
         <v>1985</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E9" s="2">
         <v>225987.60306600001</v>
@@ -12993,16 +12994,16 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C10" s="7">
         <v>1990</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E10" s="2">
         <v>215559.406682</v>
@@ -13107,16 +13108,16 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C11" s="7">
         <v>1995</v>
       </c>
       <c r="D11" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E11" s="2">
         <v>203531.29895699999</v>
@@ -13221,16 +13222,16 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C12">
         <v>2000</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E12" s="2">
         <v>191871.497348</v>
@@ -13335,16 +13336,16 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C13">
         <v>2005</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E13" s="2">
         <v>179712.17254</v>
@@ -13449,16 +13450,16 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C14">
         <v>2010</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E14" s="2">
         <v>168556.38499600001</v>
@@ -13563,16 +13564,16 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C15">
         <v>2015</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E15" s="2">
         <v>169998.90636600001</v>
@@ -13677,16 +13678,16 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C16" s="7">
         <v>1985</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E16" s="2">
         <v>244025.28</v>
@@ -13791,16 +13792,16 @@
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C17" s="7">
         <v>1990</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E17" s="2">
         <v>242271.76500000001</v>
@@ -13905,16 +13906,16 @@
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C18" s="7">
         <v>1995</v>
       </c>
       <c r="D18" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E18" s="2">
         <v>239895.76500000001</v>
@@ -14019,16 +14020,16 @@
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C19">
         <v>2000</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E19" s="2">
         <v>231647.85</v>
@@ -14133,16 +14134,16 @@
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C20">
         <v>2005</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E20" s="2">
         <v>197845.83</v>
@@ -14247,16 +14248,16 @@
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C21">
         <v>2010</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E21" s="2">
         <v>193368.55499999999</v>
@@ -14361,16 +14362,16 @@
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C22">
         <v>2015</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E22" s="2">
         <v>175085.95499999999</v>
@@ -14475,16 +14476,16 @@
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C23" s="7">
         <v>1985</v>
       </c>
       <c r="D23" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E23" s="2">
         <v>215613.81</v>
@@ -14589,16 +14590,16 @@
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C24" s="7">
         <v>1990</v>
       </c>
       <c r="D24" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E24" s="2">
         <v>208224.72</v>
@@ -14703,16 +14704,16 @@
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C25" s="7">
         <v>1995</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E25" s="2">
         <v>198331.2</v>
@@ -14817,16 +14818,16 @@
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C26">
         <v>2000</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E26" s="2">
         <v>184155.93</v>
@@ -14931,16 +14932,16 @@
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C27">
         <v>2005</v>
       </c>
       <c r="D27" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E27" s="2">
         <v>169888.23</v>
@@ -15045,16 +15046,16 @@
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C28">
         <v>2010</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E28" s="2">
         <v>174399.345</v>
@@ -15159,16 +15160,16 @@
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C29">
         <v>2015</v>
       </c>
       <c r="D29" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E29" s="2">
         <v>171939.15</v>
@@ -15273,16 +15274,16 @@
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C30" s="7">
         <v>1985</v>
       </c>
       <c r="D30" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E30" s="2">
         <v>236335.54500000001</v>
@@ -15387,16 +15388,16 @@
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C31" s="7">
         <v>1990</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E31" s="2">
         <v>229521.96</v>
@@ -15501,16 +15502,16 @@
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C32" s="7">
         <v>1995</v>
       </c>
       <c r="D32" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E32" s="2">
         <v>216679.27499999999</v>
@@ -15615,16 +15616,16 @@
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C33">
         <v>2000</v>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E33" s="2">
         <v>195863.85</v>
@@ -15729,16 +15730,16 @@
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C34">
         <v>2005</v>
       </c>
       <c r="D34" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E34" s="2">
         <v>129929.985</v>
@@ -15843,16 +15844,16 @@
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C35">
         <v>2010</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E35" s="2">
         <v>119941.33500000001</v>
@@ -15957,16 +15958,16 @@
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C36">
         <v>2015</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E36" s="2">
         <v>114476.80499999999</v>
@@ -16071,16 +16072,16 @@
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C37" s="7">
         <v>1985</v>
       </c>
       <c r="D37" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E37" s="5">
         <v>235788.48</v>
@@ -16185,16 +16186,16 @@
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C38" s="7">
         <v>1990</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E38" s="5">
         <v>228503.88</v>
@@ -16299,16 +16300,16 @@
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C39" s="7">
         <v>1995</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E39" s="5">
         <v>215717.31</v>
@@ -16413,16 +16414,16 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C40">
         <v>2000</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E40" s="5">
         <v>186367.80782099999</v>
@@ -16527,16 +16528,16 @@
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C41">
         <v>2005</v>
       </c>
       <c r="D41" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E41" s="5">
         <v>165636.94500000001</v>
@@ -16641,16 +16642,16 @@
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C42">
         <v>2010</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E42" s="5">
         <v>156989.79</v>
@@ -16755,16 +16756,16 @@
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C43">
         <v>2015</v>
       </c>
       <c r="D43" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E43" s="5">
         <v>164492.64000000001</v>
@@ -16869,16 +16870,16 @@
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C44" s="7">
         <v>1985</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E44" s="2">
         <v>227442.375</v>
@@ -16983,16 +16984,16 @@
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C45" s="7">
         <v>1990</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E45" s="2">
         <v>177051.712073</v>
@@ -17097,16 +17098,16 @@
     </row>
     <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C46" s="7">
         <v>1995</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E46" s="2">
         <v>131468.08499999999</v>
@@ -17211,16 +17212,16 @@
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="B47" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C47">
         <v>2000</v>
       </c>
       <c r="D47" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E47" s="2">
         <v>101711.34</v>
@@ -17325,16 +17326,16 @@
     </row>
     <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C48">
         <v>2005</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E48" s="2">
         <v>92836.800000000003</v>
@@ -17439,16 +17440,16 @@
     </row>
     <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C49">
         <v>2010</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E49" s="2">
         <v>97511.4</v>
@@ -17553,16 +17554,16 @@
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" t="s">
         <v>115</v>
-      </c>
-      <c r="B50" t="s">
-        <v>137</v>
       </c>
       <c r="C50">
         <v>2015</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E50" s="2">
         <v>94693.815000000002</v>
@@ -17667,16 +17668,16 @@
     </row>
     <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C51" s="7">
         <v>1985</v>
       </c>
       <c r="D51" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E51" s="2">
         <v>218658.66989700001</v>
@@ -17781,16 +17782,16 @@
     </row>
     <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B52" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C52" s="7">
         <v>1990</v>
       </c>
       <c r="D52" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E52" s="2">
         <v>202996.657289</v>
@@ -17895,16 +17896,16 @@
     </row>
     <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C53" s="7">
         <v>1995</v>
       </c>
       <c r="D53" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E53" s="2">
         <v>186165.729719</v>
@@ -18009,16 +18010,16 @@
     </row>
     <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C54">
         <v>2000</v>
       </c>
       <c r="D54" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E54" s="2">
         <v>144287.970921</v>
@@ -18123,16 +18124,16 @@
     </row>
     <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C55">
         <v>2005</v>
       </c>
       <c r="D55" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E55" s="2">
         <v>110308.00275</v>
@@ -18237,16 +18238,16 @@
     </row>
     <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C56">
         <v>2010</v>
       </c>
       <c r="D56" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E56" s="2">
         <v>111655.274238</v>
@@ -18351,16 +18352,16 @@
     </row>
     <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" t="s">
         <v>70</v>
-      </c>
-      <c r="B57" t="s">
-        <v>78</v>
       </c>
       <c r="C57">
         <v>2015</v>
       </c>
       <c r="D57" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E57" s="2">
         <v>117676.97313100001</v>
@@ -18465,16 +18466,16 @@
     </row>
     <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C58" s="7">
         <v>1985</v>
       </c>
       <c r="D58" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E58" s="2">
         <v>245391.07500000001</v>
@@ -18579,16 +18580,16 @@
     </row>
     <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C59" s="7">
         <v>1990</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E59" s="2">
         <v>240734.07</v>
@@ -18693,16 +18694,16 @@
     </row>
     <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C60" s="7">
         <v>1995</v>
       </c>
       <c r="D60" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E60" s="2">
         <v>233072.505</v>
@@ -18807,16 +18808,16 @@
     </row>
     <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C61">
         <v>2000</v>
       </c>
       <c r="D61" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E61" s="2">
         <v>225612.9</v>
@@ -18921,16 +18922,16 @@
     </row>
     <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C62">
         <v>2005</v>
       </c>
       <c r="D62" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E62" s="2">
         <v>222394.23</v>
@@ -19035,16 +19036,16 @@
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C63">
         <v>2010</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E63" s="2">
         <v>199328.04</v>
@@ -19149,16 +19150,16 @@
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C64">
         <v>2015</v>
       </c>
       <c r="D64" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E64" s="2">
         <v>198460.755</v>
@@ -19263,16 +19264,16 @@
     </row>
     <row r="65" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C65" s="7">
         <v>1985</v>
       </c>
       <c r="D65" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E65" s="2">
         <v>206934.03</v>
@@ -19377,16 +19378,16 @@
     </row>
     <row r="66" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C66" s="7">
         <v>1990</v>
       </c>
       <c r="D66" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E66" s="2">
         <v>157740.79500000001</v>
@@ -19491,16 +19492,16 @@
     </row>
     <row r="67" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C67" s="7">
         <v>1995</v>
       </c>
       <c r="D67" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E67" s="2">
         <v>121472.46</v>
@@ -19605,16 +19606,16 @@
     </row>
     <row r="68" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B68" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C68">
         <v>2000</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E68" s="2">
         <v>93623.039999999994</v>
@@ -19719,16 +19720,16 @@
     </row>
     <row r="69" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C69">
         <v>2005</v>
       </c>
       <c r="D69" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E69" s="2">
         <v>76731.12</v>
@@ -19833,16 +19834,16 @@
     </row>
     <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C70">
         <v>2010</v>
       </c>
       <c r="D70" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E70" s="2">
         <v>60901.74</v>
@@ -19947,16 +19948,16 @@
     </row>
     <row r="71" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C71">
         <v>2015</v>
       </c>
       <c r="D71" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E71" s="2">
         <v>62895.96</v>
@@ -20061,16 +20062,16 @@
     </row>
     <row r="72" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C72" s="7">
         <v>1985</v>
       </c>
       <c r="D72" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E72" s="2">
         <v>240684.21</v>
@@ -20175,16 +20176,16 @@
     </row>
     <row r="73" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C73" s="7">
         <v>1990</v>
       </c>
       <c r="D73" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E73" s="2">
         <v>237533.58</v>
@@ -20289,16 +20290,16 @@
     </row>
     <row r="74" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C74" s="7">
         <v>1995</v>
       </c>
       <c r="D74" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E74" s="2">
         <v>231074.77499999999</v>
@@ -20403,16 +20404,16 @@
     </row>
     <row r="75" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C75">
         <v>2000</v>
       </c>
       <c r="D75" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E75" s="2">
         <v>225756.45</v>
@@ -20517,16 +20518,16 @@
     </row>
     <row r="76" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C76">
         <v>2005</v>
       </c>
       <c r="D76" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E76" s="2">
         <v>213834.82500000001</v>
@@ -20631,16 +20632,16 @@
     </row>
     <row r="77" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B77" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C77">
         <v>2010</v>
       </c>
       <c r="D77" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E77" s="2">
         <v>194641.65</v>
@@ -20745,16 +20746,16 @@
     </row>
     <row r="78" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B78" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C78">
         <v>2015</v>
       </c>
       <c r="D78" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E78" s="2">
         <v>195919.02</v>
@@ -20859,16 +20860,16 @@
     </row>
     <row r="79" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C79" s="7">
         <v>1985</v>
       </c>
       <c r="D79" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E79" s="2">
         <v>234846.28</v>
@@ -20973,16 +20974,16 @@
     </row>
     <row r="80" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C80" s="7">
         <v>1990</v>
       </c>
       <c r="D80" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E80" s="2">
         <v>222443.450000001</v>
@@ -21087,16 +21088,16 @@
     </row>
     <row r="81" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B81" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C81" s="7">
         <v>1995</v>
       </c>
       <c r="D81" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E81" s="2">
         <v>188944.679999999</v>
@@ -21201,16 +21202,16 @@
     </row>
     <row r="82" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B82" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C82">
         <v>2000</v>
       </c>
       <c r="D82" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E82" s="2">
         <v>125062.069999999</v>
@@ -21315,16 +21316,16 @@
     </row>
     <row r="83" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B83" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C83">
         <v>2005</v>
       </c>
       <c r="D83" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E83" s="2">
         <v>74533.33</v>
@@ -21429,16 +21430,16 @@
     </row>
     <row r="84" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B84" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C84">
         <v>2010</v>
       </c>
       <c r="D84" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E84" s="2">
         <v>74432.17</v>
@@ -21543,16 +21544,16 @@
     </row>
     <row r="85" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B85" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C85">
         <v>2015</v>
       </c>
       <c r="D85" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E85" s="2">
         <v>62359.34</v>
@@ -21657,16 +21658,16 @@
     </row>
     <row r="86" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B86" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C86" s="7">
         <v>1985</v>
       </c>
       <c r="D86" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E86" s="2">
         <v>230003.73</v>
@@ -21771,16 +21772,16 @@
     </row>
     <row r="87" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B87" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C87" s="7">
         <v>1990</v>
       </c>
       <c r="D87" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E87" s="2">
         <v>214580.25</v>
@@ -21885,16 +21886,16 @@
     </row>
     <row r="88" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B88" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C88" s="7">
         <v>1995</v>
       </c>
       <c r="D88" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E88" s="2">
         <v>180590.58</v>
@@ -21999,16 +22000,16 @@
     </row>
     <row r="89" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B89" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C89">
         <v>2000</v>
       </c>
       <c r="D89" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E89" s="2">
         <v>178064.96</v>
@@ -22113,16 +22114,16 @@
     </row>
     <row r="90" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C90">
         <v>2005</v>
       </c>
       <c r="D90" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E90" s="2">
         <v>121745.06</v>
@@ -22227,16 +22228,16 @@
     </row>
     <row r="91" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B91" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C91">
         <v>2010</v>
       </c>
       <c r="D91" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E91" s="2">
         <v>101093.3</v>
@@ -22341,16 +22342,16 @@
     </row>
     <row r="92" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B92" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C92">
         <v>2015</v>
       </c>
       <c r="D92" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E92" s="2">
         <v>96815.42</v>
@@ -22455,16 +22456,16 @@
     </row>
     <row r="93" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="B93" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C93" s="7">
         <v>1985</v>
       </c>
       <c r="D93" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E93" s="5">
         <v>227438.595</v>
@@ -22569,16 +22570,16 @@
     </row>
     <row r="94" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="B94" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C94" s="7">
         <v>1990</v>
       </c>
       <c r="D94" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E94" s="5">
         <v>216890.46</v>
@@ -22683,16 +22684,16 @@
     </row>
     <row r="95" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="B95" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C95" s="7">
         <v>1995</v>
       </c>
       <c r="D95" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E95" s="5">
         <v>198768.78</v>
@@ -22797,16 +22798,16 @@
     </row>
     <row r="96" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="B96" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C96">
         <v>2000</v>
       </c>
       <c r="D96" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E96" s="5">
         <v>169570.71</v>
@@ -22911,16 +22912,16 @@
     </row>
     <row r="97" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="B97" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C97">
         <v>2005</v>
       </c>
       <c r="D97" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E97" s="5">
         <v>114693.84</v>
@@ -23025,16 +23026,16 @@
     </row>
     <row r="98" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="B98" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C98">
         <v>2010</v>
       </c>
       <c r="D98" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E98" s="5">
         <v>128898</v>
@@ -23139,16 +23140,16 @@
     </row>
     <row r="99" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="B99" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C99">
         <v>2015</v>
       </c>
       <c r="D99" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E99" s="5">
         <v>88674.75</v>

</xml_diff>